<commit_message>
add 3 characteristics for class card
</commit_message>
<xml_diff>
--- a/resources/cards_database/Monsters.xlsx
+++ b/resources/cards_database/Monsters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds\Desktop\Новая папка\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py progects\VldGame_\resources\cards_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E994B4-7479-4BCE-83B5-CA830AE4998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="const" sheetId="4" r:id="rId1"/>
@@ -24,15 +25,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -109,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,17 +422,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -452,7 +444,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -460,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -468,17 +460,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -490,25 +482,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -541,7 +533,7 @@
       <c r="P1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -567,7 +559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -593,7 +585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -621,7 +613,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$V$2:$V$9</formula1>
     </dataValidation>
   </dataValidations>
@@ -629,38 +621,26 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>const!$E$2:$E$4</xm:f>
           </x14:formula1>
           <xm:sqref>C13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>const!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C6</xm:sqref>
+          <xm:sqref>C5:C6 E5:E6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>const!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E5:E6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>const!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I13</xm:sqref>
+          <xm:sqref>I13 F2:F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>const!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>const!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -673,12 +653,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>